<commit_message>
Added Review Grade Filter
</commit_message>
<xml_diff>
--- a/myapp/data/smartListData.xlsx
+++ b/myapp/data/smartListData.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\viralProjects\B Tech Project\Project\CAPSLG\myapp\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08B871EF-4854-4E84-8A7A-2C85DB4A5CE1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20112" windowHeight="8016"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="154">
   <si>
     <t>College</t>
   </si>
@@ -379,12 +385,111 @@
   </si>
   <si>
     <t>Longitude</t>
+  </si>
+  <si>
+    <t>Review Grade</t>
+  </si>
+  <si>
+    <t>College code</t>
+  </si>
+  <si>
+    <t>vjti</t>
+  </si>
+  <si>
+    <t>sp</t>
+  </si>
+  <si>
+    <t>spit</t>
+  </si>
+  <si>
+    <t>ict</t>
+  </si>
+  <si>
+    <t>kjsce</t>
+  </si>
+  <si>
+    <t>kjit</t>
+  </si>
+  <si>
+    <t>vik</t>
+  </si>
+  <si>
+    <t>sa</t>
+  </si>
+  <si>
+    <t>dbit</t>
+  </si>
+  <si>
+    <t>djs</t>
+  </si>
+  <si>
+    <t>fcr</t>
+  </si>
+  <si>
+    <t>ss</t>
+  </si>
+  <si>
+    <t>rgit</t>
+  </si>
+  <si>
+    <t>rcr</t>
+  </si>
+  <si>
+    <t>bvc</t>
+  </si>
+  <si>
+    <t>dmc</t>
+  </si>
+  <si>
+    <t>afrc</t>
+  </si>
+  <si>
+    <t>kc</t>
+  </si>
+  <si>
+    <t>kgc</t>
+  </si>
+  <si>
+    <t>lti</t>
+  </si>
+  <si>
+    <t>mgm</t>
+  </si>
+  <si>
+    <t>pvp</t>
+  </si>
+  <si>
+    <t>pit</t>
+  </si>
+  <si>
+    <t>rait</t>
+  </si>
+  <si>
+    <t>jc</t>
+  </si>
+  <si>
+    <t>sies</t>
+  </si>
+  <si>
+    <t>sfit</t>
+  </si>
+  <si>
+    <t>tec</t>
+  </si>
+  <si>
+    <t>tcet</t>
+  </si>
+  <si>
+    <t>tse</t>
+  </si>
+  <si>
+    <t>vit</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -434,7 +539,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -466,11 +571,56 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFEBEBEB"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFEBEBEB"/>
+      </left>
+      <right style="thick">
+        <color rgb="FFEBEBEB"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFEBEBEB"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -490,7 +640,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -499,8 +649,17 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -511,6 +670,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -559,7 +721,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -592,9 +754,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -627,6 +806,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -802,677 +998,872 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B3" sqref="B3:B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="81.88671875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="83.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="44.44140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="27.44140625" customWidth="1"/>
-    <col min="7" max="7" width="28.109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="81.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" style="1" customWidth="1"/>
+    <col min="3" max="4" width="81.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="83.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="44.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="27.42578125" customWidth="1"/>
+    <col min="8" max="8" width="28.140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I1" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C3" s="1">
         <v>19.0222181</v>
       </c>
-      <c r="C3" s="1">
+      <c r="D3" s="1">
         <v>72.856121199999905</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="F3" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I3" s="10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C4" s="2">
         <v>19.1238086</v>
       </c>
-      <c r="C4" s="2">
+      <c r="D4" s="2">
         <v>72.836138800000001</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I4" s="10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C5" s="3">
         <v>19.123177599999899</v>
       </c>
-      <c r="C5" s="3">
+      <c r="D5" s="3">
         <v>72.836115399999898</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I5" s="10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C6" s="1">
         <v>19.023919200000002</v>
       </c>
-      <c r="C6" s="1">
+      <c r="D6" s="1">
         <v>72.857520699999995</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="F6" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="G6" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I6" s="10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C7" s="3">
         <v>19.072673999999999</v>
       </c>
-      <c r="C7" s="3">
+      <c r="D7" s="3">
         <v>72.900698899999895</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="F7" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="G7" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I7" s="10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C8" s="3">
         <v>19.046146</v>
       </c>
-      <c r="C8" s="3">
+      <c r="D8" s="3">
         <v>72.871042999999901</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="F8" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="G8" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I8" s="10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C9" s="3">
         <v>19.045338300000001</v>
       </c>
-      <c r="C9" s="3">
+      <c r="D9" s="3">
         <v>72.888943100000006</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="F9" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="G9" s="1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I9" s="10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C10" s="3">
         <v>19.0482157</v>
       </c>
-      <c r="C10" s="3">
+      <c r="D10" s="3">
         <v>72.911658099999997</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="G10" s="1" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I10" s="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C11" s="3">
         <v>19.081253199999999</v>
       </c>
-      <c r="C11" s="3">
+      <c r="D11" s="3">
         <v>72.888596099999901</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="F11" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="G11" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I11" s="11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C12" s="3">
         <v>19.107105900000001</v>
       </c>
-      <c r="C12" s="3">
+      <c r="D12" s="3">
         <v>72.837107399999994</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="G12" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="G12" s="5"/>
-    </row>
-    <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H12" s="5"/>
+      <c r="I12" s="12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C13" s="3">
         <v>19.044497</v>
       </c>
-      <c r="C13" s="3">
+      <c r="D13" s="3">
         <v>72.8204534999999</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="F13" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="G13" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="G13"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H13"/>
+      <c r="I13" s="13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C14" s="3">
         <v>18.968510299999998</v>
       </c>
-      <c r="C14" s="3">
+      <c r="D14" s="3">
         <v>72.831024899999903</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="G14" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="G14"/>
-    </row>
-    <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H14"/>
+      <c r="I14" s="13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C15" s="3">
         <v>19.121276099999999</v>
       </c>
-      <c r="C15" s="3">
+      <c r="D15" s="3">
         <v>72.823696100000006</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="G15" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I15" s="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C16" s="3">
         <v>19.066676999999999</v>
       </c>
-      <c r="C16" s="3">
+      <c r="D16" s="3">
         <v>72.824806099999904</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="F16" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="F16" s="10" t="s">
+      <c r="G16" s="1" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I16" s="10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="C17" s="4">
         <v>19.026493299999998</v>
       </c>
-      <c r="C17" s="4">
+      <c r="D17" s="4">
         <v>73.055066399999902</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="F17" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="F17" s="10" t="s">
+      <c r="G17" s="1" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I17" s="10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C18" s="3">
         <v>19.160322000000001</v>
       </c>
-      <c r="C18" s="3">
+      <c r="D18" s="3">
         <v>72.995568000000006</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="F18" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="F18" s="10" t="s">
+      <c r="G18" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="H18" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I18" s="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C19" s="3">
         <v>19.075512700000001</v>
       </c>
-      <c r="C19" s="3">
+      <c r="D19" s="3">
         <v>72.991704299999995</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F19" s="10" t="s">
+      <c r="G19" s="1" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I19" s="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C20" s="3">
         <v>19.179929699999999</v>
       </c>
-      <c r="C20" s="3">
+      <c r="D20" s="3">
         <v>72.980271599999895</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="G20" s="1" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I20" s="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C21" s="3">
         <v>18.915902899999999</v>
       </c>
-      <c r="C21" s="3">
+      <c r="D21" s="3">
         <v>73.343190999999905</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I21" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C22" s="3">
         <v>19.105774</v>
       </c>
-      <c r="C22" s="3">
+      <c r="D22" s="3">
         <v>73.007290900000001</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="H22" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I22" s="10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C23" s="3">
         <v>19.016387300000002</v>
       </c>
-      <c r="C23" s="3">
+      <c r="D23" s="3">
         <v>73.104657799999998</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E23" s="6" t="s">
+      <c r="F23" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="F23" s="10" t="s">
+      <c r="G23" s="1" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I23" s="10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C24" s="3">
         <v>19.050429300000001</v>
       </c>
-      <c r="C24" s="3">
+      <c r="D24" s="3">
         <v>72.878434400000003</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E24" s="9" t="s">
+      <c r="F24" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="F24" s="10" t="s">
+      <c r="G24" s="1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I24" s="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B25" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C25" s="3">
         <v>18.990200999999999</v>
       </c>
-      <c r="C25" s="3">
+      <c r="D25" s="3">
         <v>73.127670099999904</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="F25" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="F25" s="10" t="s">
+      <c r="G25" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I25" s="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B26" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C26" s="3">
         <v>19.044384699999998</v>
       </c>
-      <c r="C26" s="3">
+      <c r="D26" s="3">
         <v>73.025700599999894</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="F26" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="F26" s="10" t="s">
+      <c r="G26" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="G26" s="1" t="s">
+      <c r="H26" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I26" s="10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B27" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C27" s="3">
         <v>19.197952399999998</v>
       </c>
-      <c r="C27" s="3">
+      <c r="D27" s="3">
         <v>73.108284099999906</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I27" s="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B28" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C28" s="3">
         <v>19.042812999999999</v>
       </c>
-      <c r="C28" s="3">
+      <c r="D28" s="3">
         <v>73.023077999999899</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="E28" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="F28" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="F28" s="10" t="s">
+      <c r="G28" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="G28" s="1" t="s">
+      <c r="H28" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I28" s="10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B29" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C29" s="3">
         <v>19.243552600000001</v>
       </c>
-      <c r="C29" s="3">
+      <c r="D29" s="3">
         <v>72.855797100000004</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="E29" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="F29" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="F29" s="10" t="s">
+      <c r="G29" s="1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I29" s="10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B30" s="3">
+      <c r="B30" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C30" s="3">
         <v>19.029648900000002</v>
       </c>
-      <c r="C30" s="3">
+      <c r="D30" s="3">
         <v>73.016669299999904</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="F30" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="F30" s="10" t="s">
+      <c r="G30" s="1" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I30" s="10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B31" s="3">
+      <c r="B31" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C31" s="3">
         <v>19.206134200000001</v>
       </c>
-      <c r="C31" s="3">
+      <c r="D31" s="3">
         <v>72.874532400000007</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="E31" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E31" s="6" t="s">
+      <c r="F31" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="F31" s="10" t="s">
+      <c r="G31" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="G31" s="1" t="s">
+      <c r="H31" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I31" s="10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B32" s="3">
+      <c r="B32" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C32" s="3">
         <v>19.064464699999998</v>
       </c>
-      <c r="C32" s="3">
+      <c r="D32" s="3">
         <v>72.835860199999999</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="E32" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E32" s="6" t="s">
+      <c r="F32" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="F32" s="10" t="s">
+      <c r="G32" s="1" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I32" s="10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B33" s="3">
+      <c r="B33" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C33" s="3">
         <v>19.0215885</v>
       </c>
-      <c r="C33" s="3">
+      <c r="D33" s="3">
         <v>72.870736299999905</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="E33" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E33" s="9"/>
-      <c r="G33" s="1" t="s">
+      <c r="F33" s="9"/>
+      <c r="H33" s="1" t="s">
         <v>44</v>
+      </c>
+      <c r="I33" s="10">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1482,24 +1873,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>